<commit_message>
List filters and Debounce search
</commit_message>
<xml_diff>
--- a/Backend/static/export_temp/exported_lists.xlsx
+++ b/Backend/static/export_temp/exported_lists.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -465,82 +465,22 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t xml:space="preserve">New List </t>
+          <t>Nihar</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>pending</t>
+          <t>active</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">helo new list is here </t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>18</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>List 826</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>active</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>description for 826</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>12</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Nihar</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>active</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
         <is>
           <t xml:space="preserve">Description for nihar list and it is list desc
 </t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>19</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Fifth Reocrd</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>active</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>it is for 5th</t>
         </is>
       </c>
     </row>

</xml_diff>